<commit_message>
Make an empty project structure
</commit_message>
<xml_diff>
--- a/BowlingAlly.xlsx
+++ b/BowlingAlly.xlsx
@@ -5,15 +5,16 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AELLEUC5\Desktop\BowlingAlly\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AELLEUC5\Desktop\BowlingAlly\BowlingAlly\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54EBA9A9-E82A-46B5-B808-7B9FAF30F97C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE6AC71A-77E8-474B-B586-435B09ABE12C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Design " sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="51">
   <si>
     <t>task</t>
   </si>
@@ -48,12 +49,6 @@
     <t>Create packages</t>
   </si>
   <si>
-    <t xml:space="preserve">Create foo function and have a code tha compile </t>
-  </si>
-  <si>
-    <t xml:space="preserve">create testes for every foo function </t>
-  </si>
-  <si>
     <t xml:space="preserve">Create function to calcule score of a given game </t>
   </si>
   <si>
@@ -88,16 +83,140 @@
   </si>
   <si>
     <t>end</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Make a nemurcal design </t>
+  </si>
+  <si>
+    <t xml:space="preserve">class name </t>
+  </si>
+  <si>
+    <t>atribute</t>
+  </si>
+  <si>
+    <t>methodes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Player </t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Name </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Game </t>
+  </si>
+  <si>
+    <t xml:space="preserve">score </t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t xml:space="preserve">frame  </t>
+  </si>
+  <si>
+    <t>Current round</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Integer </t>
+  </si>
+  <si>
+    <t xml:space="preserve">String </t>
+  </si>
+  <si>
+    <t>Roll1</t>
+  </si>
+  <si>
+    <t>Roll2</t>
+  </si>
+  <si>
+    <t>SetRoll</t>
+  </si>
+  <si>
+    <t>Game</t>
+  </si>
+  <si>
+    <t xml:space="preserve">array of 10 frames </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Get previous game Type </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Get actual frame number </t>
+  </si>
+  <si>
+    <t xml:space="preserve">get Actual frame number </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Objects </t>
+  </si>
+  <si>
+    <t>Types</t>
+  </si>
+  <si>
+    <t>Roll_type</t>
+  </si>
+  <si>
+    <t>Game_type</t>
+  </si>
+  <si>
+    <t>attribute</t>
+  </si>
+  <si>
+    <t>Classes</t>
+  </si>
+  <si>
+    <t>New types</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Integer between 0 and 10 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">NB: every think must be worked before every commit </t>
+  </si>
+  <si>
+    <t xml:space="preserve">create testes environment for every foo function </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00B0F0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF7030A0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="4"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -123,9 +242,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -406,10 +529,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="C3:I18"/>
+  <dimension ref="C3:I20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N16" sqref="N16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E11" sqref="E11:E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -421,15 +544,20 @@
   <sheetData>
     <row r="3" spans="3:9" x14ac:dyDescent="0.3">
       <c r="I3" t="s">
-        <v>11</v>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="I4" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="5" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E5" t="s">
         <v>0</v>
@@ -458,106 +586,313 @@
         <v>12</v>
       </c>
       <c r="I6" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C7" s="1">
+        <v>0.22500000000000001</v>
+      </c>
       <c r="D7" s="1">
         <v>0.21666666666666667</v>
       </c>
       <c r="E7">
         <v>1</v>
       </c>
+      <c r="F7">
+        <v>12</v>
+      </c>
       <c r="I7" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="8" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="E8">
-        <v>2</v>
+      <c r="C8" s="1">
+        <v>0.23611111111111113</v>
+      </c>
+      <c r="D8" s="1">
+        <v>0.22500000000000001</v>
+      </c>
+      <c r="F8">
+        <v>16</v>
       </c>
       <c r="I8" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="3:9" x14ac:dyDescent="0.3">
       <c r="E9">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I9" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="E10">
-        <v>4</v>
-      </c>
-      <c r="I10" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="11" spans="3:9" x14ac:dyDescent="0.3">
       <c r="E11">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="I11" t="s">
-        <v>9</v>
+        <v>50</v>
       </c>
     </row>
     <row r="12" spans="3:9" x14ac:dyDescent="0.3">
       <c r="E12">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="I12" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="13" spans="3:9" x14ac:dyDescent="0.3">
       <c r="E13">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="I13" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="14" spans="3:9" x14ac:dyDescent="0.3">
       <c r="E14">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="I14" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="15" spans="3:9" x14ac:dyDescent="0.3">
       <c r="E15">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="I15" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="16" spans="3:9" x14ac:dyDescent="0.3">
       <c r="E16">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="I16" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="17" spans="5:9" x14ac:dyDescent="0.3">
       <c r="E17">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="I17" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="18" spans="5:9" x14ac:dyDescent="0.3">
       <c r="E18">
+        <v>10</v>
+      </c>
+      <c r="I18" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="19" spans="5:9" x14ac:dyDescent="0.3">
+      <c r="E19">
+        <v>11</v>
+      </c>
+      <c r="I19" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="20" spans="5:9" x14ac:dyDescent="0.3">
+      <c r="E20">
         <v>12</v>
       </c>
-      <c r="I18" t="s">
-        <v>17</v>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{044D0F4C-1344-4C6E-9AE7-7BF6F9E96A96}">
+  <dimension ref="A2:P15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="T22" sqref="T22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="6" max="6" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.77734375" customWidth="1"/>
+    <col min="9" max="9" width="5.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="4.5546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="22.109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="22.109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="E2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="F3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="J3" t="s">
+        <v>20</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="N3" t="s">
+        <v>20</v>
+      </c>
+      <c r="O3" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="F4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G4" t="s">
+        <v>24</v>
+      </c>
+      <c r="H4" t="s">
+        <v>22</v>
+      </c>
+      <c r="I4" t="s">
+        <v>24</v>
+      </c>
+      <c r="J4" t="s">
+        <v>21</v>
+      </c>
+      <c r="K4" t="s">
+        <v>24</v>
+      </c>
+      <c r="L4" t="s">
+        <v>22</v>
+      </c>
+      <c r="M4" t="s">
+        <v>24</v>
+      </c>
+      <c r="N4" t="s">
+        <v>21</v>
+      </c>
+      <c r="O4" t="s">
+        <v>24</v>
+      </c>
+      <c r="P4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="G5" t="s">
+        <v>32</v>
+      </c>
+      <c r="H5" t="s">
+        <v>28</v>
+      </c>
+      <c r="I5" t="s">
+        <v>28</v>
+      </c>
+      <c r="J5" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="K5" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="L5" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="N5" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="O5" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="P5" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A6" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="J6" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="K6" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="P6" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A7" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="G7" t="s">
+        <v>31</v>
+      </c>
+      <c r="P7" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="F8" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="G8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="E13" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="F14" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="G14" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="F15" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="G15" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Implement Function setRoll <Frame>
</commit_message>
<xml_diff>
--- a/BowlingAlly.xlsx
+++ b/BowlingAlly.xlsx
@@ -8,25 +8,36 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AELLEUC5\Desktop\BowlingAlly\BowlingAlly\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6822E0A9-F4AB-4E93-97D0-90BDB92AAE97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A7A4778-8244-47A3-83BF-8EF84EFA328E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38400" yWindow="8010" windowWidth="14400" windowHeight="7560" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="1728" windowWidth="9216" windowHeight="2616" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Design " sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="55">
   <si>
     <t>task</t>
   </si>
@@ -178,7 +189,19 @@
     <t xml:space="preserve">Create empty project structure </t>
   </si>
   <si>
-    <t>create skeletton environment</t>
+    <t>git add</t>
+  </si>
+  <si>
+    <t>create skeletton environment part 1</t>
+  </si>
+  <si>
+    <t>create skeletton environment part 2</t>
+  </si>
+  <si>
+    <t>create skeletton environment part 3</t>
+  </si>
+  <si>
+    <t>Implement Function setRoll &lt;Frame&gt;</t>
   </si>
 </sst>
 </file>
@@ -529,10 +552,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="C3:I20"/>
+  <dimension ref="B3:I23"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -542,17 +565,17 @@
     <col min="9" max="9" width="64.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:9" x14ac:dyDescent="0.3">
       <c r="I3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:9" x14ac:dyDescent="0.3">
       <c r="I4" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="5" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:9" x14ac:dyDescent="0.3">
       <c r="C5" t="s">
         <v>17</v>
       </c>
@@ -575,7 +598,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D6" s="1">
         <v>0.20833333333333334</v>
       </c>
@@ -589,7 +612,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:9" x14ac:dyDescent="0.3">
       <c r="C7" s="1">
         <v>0.22500000000000001</v>
       </c>
@@ -606,7 +629,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:9" x14ac:dyDescent="0.3">
       <c r="C8" s="1">
         <v>0.23611111111111113</v>
       </c>
@@ -620,7 +643,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:9" x14ac:dyDescent="0.3">
       <c r="C9" s="1">
         <v>0.24444444444444446</v>
       </c>
@@ -634,55 +657,84 @@
         <v>49</v>
       </c>
     </row>
-    <row r="11" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="C11" s="1">
+        <v>0.28472222222222221</v>
+      </c>
       <c r="D11" s="1">
         <v>0.26180555555555557</v>
       </c>
       <c r="E11">
         <v>3</v>
       </c>
+      <c r="F11">
+        <v>23</v>
+      </c>
       <c r="I11" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="12" spans="3:9" x14ac:dyDescent="0.3">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="12" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B12">
+        <f>SUM(F6:F25)</f>
+        <v>322</v>
+      </c>
+      <c r="C12" s="1">
+        <v>0.33888888888888885</v>
+      </c>
+      <c r="D12" s="1">
+        <v>0.29166666666666669</v>
+      </c>
       <c r="E12">
         <v>4</v>
       </c>
+      <c r="F12">
+        <v>68</v>
+      </c>
       <c r="I12" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="13" spans="3:9" x14ac:dyDescent="0.3">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B13">
+        <f>B12/60</f>
+        <v>5.3666666666666663</v>
+      </c>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
       <c r="E13">
         <v>5</v>
       </c>
+      <c r="F13">
+        <f>15+18+41+15+60</f>
+        <v>149</v>
+      </c>
       <c r="I13" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="14" spans="3:9" x14ac:dyDescent="0.3">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="14" spans="2:9" x14ac:dyDescent="0.3">
       <c r="E14">
         <v>6</v>
       </c>
+      <c r="F14">
+        <v>30</v>
+      </c>
       <c r="I14" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="15" spans="3:9" x14ac:dyDescent="0.3">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="15" spans="2:9" x14ac:dyDescent="0.3">
       <c r="E15">
         <v>7</v>
       </c>
-      <c r="I15" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="16" spans="3:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="16" spans="2:9" x14ac:dyDescent="0.3">
       <c r="E16">
         <v>8</v>
       </c>
       <c r="I16" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="17" spans="5:9" x14ac:dyDescent="0.3">
@@ -690,7 +742,7 @@
         <v>9</v>
       </c>
       <c r="I17" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row r="18" spans="5:9" x14ac:dyDescent="0.3">
@@ -698,7 +750,7 @@
         <v>10</v>
       </c>
       <c r="I18" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
     <row r="19" spans="5:9" x14ac:dyDescent="0.3">
@@ -706,12 +758,30 @@
         <v>11</v>
       </c>
       <c r="I19" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="20" spans="5:9" x14ac:dyDescent="0.3">
       <c r="E20">
         <v>12</v>
+      </c>
+      <c r="I20" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="21" spans="5:9" x14ac:dyDescent="0.3">
+      <c r="I21" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="22" spans="5:9" x14ac:dyDescent="0.3">
+      <c r="I22" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="23" spans="5:9" x14ac:dyDescent="0.3">
+      <c r="I23" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -721,9 +791,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{044D0F4C-1344-4C6E-9AE7-7BF6F9E96A96}">
-  <dimension ref="A2:P15"/>
+  <dimension ref="A2:T22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+    <sheetView topLeftCell="E1" workbookViewId="0">
       <selection activeCell="T22" sqref="T22"/>
     </sheetView>
   </sheetViews>
@@ -904,6 +974,11 @@
         <v>47</v>
       </c>
     </row>
+    <row r="22" spans="20:20" x14ac:dyDescent="0.3">
+      <c r="T22" t="s">
+        <v>50</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>